<commit_message>
added buffer cap, 100ohm resistor
</commit_message>
<xml_diff>
--- a/Acoustics_BOM_2-16.xlsx
+++ b/Acoustics_BOM_2-16.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\URC\ALTIUM PROJECTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ilena Johnson\Documents\URC\PCBs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F50AACB7-BAC8-47C3-9231-BE3DE8D7C411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D42675D-2D1A-4084-AF1B-CAE39F67F1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{01697AEB-5223-423A-A058-60F9F89EA19A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{01697AEB-5223-423A-A058-60F9F89EA19A}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoustics" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="154">
   <si>
     <t>Designator</t>
   </si>
@@ -461,6 +461,45 @@
   </si>
   <si>
     <t>Quantity to Purchase</t>
+  </si>
+  <si>
+    <t>C-PWR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">220 uF buffering cap </t>
+  </si>
+  <si>
+    <t>220 uF</t>
+  </si>
+  <si>
+    <t>1206-C</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>RG</t>
+  </si>
+  <si>
+    <t>100 ohm resistor switch to gnd</t>
+  </si>
+  <si>
+    <t>0805 (1206 Metric)</t>
+  </si>
+  <si>
+    <t>GRM31CR60J227ME11L</t>
+  </si>
+  <si>
+    <t>https://search.murata.co.jp/Ceramy/image/img/A01X/G101/ENG/GRM31CR60J227ME11-01.pdf</t>
+  </si>
+  <si>
+    <t>Yageo</t>
+  </si>
+  <si>
+    <t>AC0805FR-10100RL</t>
+  </si>
+  <si>
+    <t>https://www.yageo.com/upload/media/product/productsearch/datasheet/rchip/PYu-AC_51_RoHS_L_8.pdf</t>
   </si>
 </sst>
 </file>
@@ -500,7 +539,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -523,12 +562,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -538,6 +588,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -853,27 +904,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C644D028-A5D6-4B62-AA4B-06EEB30B9CB5}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="53.28515625" customWidth="1"/>
-    <col min="2" max="3" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="53.33203125" customWidth="1"/>
+    <col min="2" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="89" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="168.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="168.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -908,7 +959,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
@@ -941,7 +992,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -949,7 +1000,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C27" si="0">ROUNDUP(B3*1.5,2)</f>
+        <f t="shared" ref="C3:C21" si="0">ROUNDUP(B3*1.5,2)</f>
         <v>18</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -977,7 +1028,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>25</v>
       </c>
@@ -1011,7 +1062,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>32</v>
       </c>
@@ -1045,7 +1096,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>37</v>
       </c>
@@ -1079,7 +1130,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1113,7 +1164,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -1147,7 +1198,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>48</v>
       </c>
@@ -1181,7 +1232,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>53</v>
       </c>
@@ -1215,7 +1266,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>58</v>
       </c>
@@ -1249,7 +1300,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>66</v>
       </c>
@@ -1279,7 +1330,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -1313,7 +1364,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>73</v>
       </c>
@@ -1347,7 +1398,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>78</v>
       </c>
@@ -1381,7 +1432,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1415,7 +1466,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>86</v>
       </c>
@@ -1449,7 +1500,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>90</v>
       </c>
@@ -1483,7 +1534,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>94</v>
       </c>
@@ -1519,7 +1570,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>102</v>
       </c>
@@ -1554,7 +1605,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>107</v>
       </c>
@@ -1586,7 +1637,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>108</v>
       </c>
@@ -1619,7 +1670,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>113</v>
       </c>
@@ -1652,7 +1703,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>118</v>
       </c>
@@ -1685,7 +1736,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>124</v>
       </c>
@@ -1708,7 +1759,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>126</v>
       </c>
@@ -1741,7 +1792,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>130</v>
       </c>
@@ -1770,6 +1821,58 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1" t="s">
         <v>139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="I28" t="s">
+        <v>149</v>
+      </c>
+      <c r="K28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="B29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="G29" t="s">
+        <v>148</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" t="s">
+        <v>152</v>
+      </c>
+      <c r="K29" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>